<commit_message>
Switching test engine for tests.
</commit_message>
<xml_diff>
--- a/POM/src/main/java/SearchTerm.xlsx
+++ b/POM/src/main/java/SearchTerm.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ADE743-C152-418B-9199-2175F881A423}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C7FD13-A945-4669-9470-C0C68166112F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,13 @@
     <t>SearchTerm</t>
   </si>
   <si>
-    <t>Sachin Tendulkar</t>
+    <t>Amazon</t>
   </si>
   <si>
-    <t>Sourav Ganguly</t>
+    <t>Ebay</t>
   </si>
   <si>
-    <t>Rahul Dravid</t>
+    <t>Wish</t>
   </si>
 </sst>
 </file>
@@ -370,15 +370,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -386,7 +386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -394,7 +394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -402,7 +402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>

</xml_diff>